<commit_message>
changed feture file and runner class and hooks class
</commit_message>
<xml_diff>
--- a/TechMApp/src/com/resources/testData/TestData-seleniumframework.xlsx
+++ b/TechMApp/src/com/resources/testData/TestData-seleniumframework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14430" windowHeight="2655" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="2985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignInSignOut" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:I6"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -44,30 +44,6 @@
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>subject</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>order_reference</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>Customer service</t>
-  </si>
-  <si>
-    <t>abc@123.com</t>
-  </si>
-  <si>
-    <t>Testmessage1</t>
-  </si>
-  <si>
-    <t>abc123</t>
   </si>
   <si>
     <t>Mahesh.ahsajjan@gmail.com</t>
@@ -147,17 +123,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -467,7 +439,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +515,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +526,7 @@
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -568,56 +540,27 @@
       <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="G1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G2"/>
     </row>
     <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="6"/>
+      <c r="G3" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>